<commit_message>
Adding the setup doc
</commit_message>
<xml_diff>
--- a/Chef_Training.xlsx
+++ b/Chef_Training.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cognizant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nokram\Documents\ChefTraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Workstation Setup</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>(Ubuntu 16)</t>
+  </si>
+  <si>
+    <t>Verify SSH client</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +554,7 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -609,7 +612,9 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>